<commit_message>
refactor to classes + fetching by chunks
</commit_message>
<xml_diff>
--- a/files/example.xlsx
+++ b/files/example.xlsx
@@ -376,7 +376,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -391,31 +391,255 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>6632801</v>
+        <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>https://masterwatt.ru/catalog/vodonagrevateli-kosvennogo-nagreva/vodonagrevatel-hrs-321/</v>
+        <v>https://masterwatt.ru/catalog/komplektuyushchie-i-zapchasti-k-kotlam/komnatnyy-regulyator-thermolink-b-ebus-24-v-montazh-naruzhny/</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>6632801</v>
+        <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>https://masterwatt.ru/catalog/vodonagrevateli-kosvennogo-nagreva/vodonagrevatel-hrs-321/</v>
+        <v>https://masterwatt.ru/catalog/komplektuyushchie-i-zapchasti-k-kotlam/komnatnyy-regulyator-thermolink-b-ebus-24-v-montazh-naruzhny/</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>6632801</v>
+        <v>3</v>
       </c>
       <c r="B4" t="str">
-        <v>https://masterwatt.ru/catalog/vodonagrevateli-kosvennogo-nagreva/vodonagrevatel-hrs-321/</v>
+        <v>https://masterwatt.ru/catalog/komplektuyushchie-i-zapchasti-k-kotlam/komnatnyy-regulyator-thermolink-b-ebus-24-v-montazh-naruzhny/</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="str">
+        <v>https://masterwatt.ru/catalog/komplektuyushchie-i-zapchasti-k-kotlam/komnatnyy-regulyator-thermolink-b-ebus-24-v-montazh-naruzhny/</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="str">
+        <v>https://masterwatt.ru/catalog/komplektuyushchie-i-zapchasti-k-kotlam/komnatnyy-regulyator-thermolink-b-ebus-24-v-montazh-naruzhny/</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="str">
+        <v>https://masterwatt.ru/catalog/komplektuyushchie-i-zapchasti-k-kotlam/komnatnyy-regulyator-thermolink-b-ebus-24-v-montazh-naruzhny/</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="str">
+        <v>https://masterwatt.ru/catalog/komplektuyushchie-i-zapchasti-k-kotlam/komplekt-perevoda-na-szhizhennyy-gaz-dlya-kotla-gepard-12-i-/</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="str">
+        <v>https://masterwatt.ru/catalog/prinadlezhnosti-dlya-sistem-podderzhaniya-davleniya-i-podpit/plata-plavnogo-puska-dvukh-nasosov-sanftanlaufplatine-2-pump/</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="str">
+        <v>https://masterwatt.ru/catalog/komplektuyushchie-i-zapchasti-k-kotlam/komnatnyy-regulyator-thermolink-b-ebus-24-v-montazh-naruzhny/</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="str">
+        <v>https://masterwatt.ru/catalog/prinadlezhnosti-dlya-sistem-podderzhaniya-davleniya-i-podpit/datchik-urovnya-zhidkosti-v-emkostyakh-vg-rg-gg-4-20-ma-0-10~1/</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="str">
+        <v>https://masterwatt.ru/catalog/komplektuyushchie-i-zapchasti-k-kotlam/komplekt-perevoda-na-szhizhennyy-gaz-dlya-kotla-gepard-12-i-/</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="str">
+        <v>https://masterwatt.ru/catalog/komplektuyushchie-i-zapchasti-k-kotlam/komplekt-perevoda-na-szhizhennyy-gaz-dlya-kotla-pantera-12-k/</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="str">
+        <v>https://masterwatt.ru/catalog/vodorozetki/ugolnik-ustanovochnyy-gx-20x1-2-f-45-mm/</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="str">
+        <v>https://masterwatt.ru/catalog/rasshiritelnye-baki/rasshiritelnyy-bak-de-6000-s-16-dn-65-pn-16-siniy-c-t-v-cert/</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>asd15</v>
+      </c>
+      <c r="B16" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="str">
+        <v>https://masterwatt.ru/catalog/komplektuyushchie-i-zapchasti-k-kotlam/komplekt-perevoda-na-szhizhennyy-gaz-dlya-kotla-gepard-12-i-/</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="str">
+        <v>https://masterwatt.ru/catalog/komplektuyushchie-i-zapchasti-k-kotlam/datchik-boylera-ntc-dlya-kotlov-pantera-12-kto-25-kto-25-koo/</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="str">
+        <v>https://masterwatt.ru/catalog/separatory/separator-gryazi-i-shlama-reflex-exdirt-r-hc-s-d-200-16-bar-/</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="str">
+        <v>https://masterwatt.ru/catalog/komplektuyushchie-i-zapchasti-k-kotlam/komnatnyy-regulyator-thermolink-b-ebus-24-v-montazh-naruzhny/</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="str">
+        <v>https://masterwatt.ru/catalog/komplektuyushchie-i-zapchasti-k-kotlam/komnatnyy-regulyator-thermolink-b-ebus-24-v-montazh-naruzhny/</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="str">
+        <v>https://masterwatt.ru/catalog/komplektuyushchie-i-zapchasti-k-kotlam/komplekt-perevoda-na-szhizhennyy-gaz-dlya-kotla-gepard-12-i-/</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="str">
+        <v>https://masterwatt.ru/catalog/prinadlezhnosti-dlya-sistem-podderzhaniya-davleniya-i-podpit/vakuumnyy-deaerator-servitec-60-t-control-touch/</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="str">
+        <v>https://masterwatt.ru/catalog/komplektuyushchie-i-zapchasti-k-kotlam/komplekt-perevoda-na-szhizhennyy-gaz-dlya-kotla-gepard-12-i-/</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="str">
+        <v>https://masterwatt.ru/catalog/komplektuyushchie-i-zapchasti-k-kotlam/komnatnyy-regulyator-thermolink-b-ebus-24-v-montazh-naruzhny/</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26" t="str">
+        <v>https://masterwatt.ru/catalog/komplektuyushchie-i-zapchasti-k-kotlam/komnatnyy-regulyator-thermolink-b-ebus-24-v-montazh-naruzhny/</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27">
+        <v>3</v>
+      </c>
+      <c r="B27" t="str">
+        <v>https://masterwatt.ru/catalog/komplektuyushchie-i-zapchasti-k-kotlam/komnatnyy-regulyator-thermolink-b-ebus-24-v-montazh-naruzhny/</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28">
+        <v>4</v>
+      </c>
+      <c r="B28" t="str">
+        <v>https://masterwatt.ru/catalog/komplektuyushchie-i-zapchasti-k-kotlam/komnatnyy-regulyator-thermolink-b-ebus-24-v-montazh-naruzhny/</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29" t="str">
+        <v>https://masterwatt.ru/catalog/komplektuyushchie-i-zapchasti-k-kotlam/komnatnyy-regulyator-thermolink-b-ebus-24-v-montazh-naruzhny/</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30">
+        <v>6</v>
+      </c>
+      <c r="B30" t="str">
+        <v>https://masterwatt.ru/catalog/komplektuyushchie-i-zapchasti-k-kotlam/komnatnyy-regulyator-thermolink-b-ebus-24-v-montazh-naruzhny/</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31">
+        <v>7</v>
+      </c>
+      <c r="B31" t="str">
+        <v>https://masterwatt.ru/catalog/komplektuyushchie-i-zapchasti-k-kotlam/komplekt-perevoda-na-szhizhennyy-gaz-dlya-kotla-gepard-12-i-/</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32">
+        <v>8</v>
+      </c>
+      <c r="B32" t="str">
+        <v>https://masterwatt.ru/catalog/prinadlezhnosti-dlya-sistem-podderzhaniya-davleniya-i-podpit/plata-plavnogo-puska-dvukh-nasosov-sanftanlaufplatine-2-pump/</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B32"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>